<commit_message>
testprep: fix: updated xls and defaulting userstatus to empty string
</commit_message>
<xml_diff>
--- a/app/src/main/res/raw/qbank_v1.xlsx
+++ b/app/src/main/res/raw/qbank_v1.xlsx
@@ -2043,7 +2043,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N100"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N1" sqref="N1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2142,9 +2144,7 @@
       <c r="M2" s="6">
         <v>1</v>
       </c>
-      <c r="N2" s="6">
-        <v>0</v>
-      </c>
+      <c r="N2" s="6"/>
     </row>
     <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3" s="7" t="s">
@@ -2186,9 +2186,7 @@
       <c r="M3" s="6">
         <v>2</v>
       </c>
-      <c r="N3" s="6">
-        <v>0</v>
-      </c>
+      <c r="N3" s="6"/>
     </row>
     <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4" s="7" t="s">
@@ -2230,9 +2228,7 @@
       <c r="M4" s="6">
         <v>3</v>
       </c>
-      <c r="N4" s="6">
-        <v>0</v>
-      </c>
+      <c r="N4" s="6"/>
     </row>
     <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5" s="7" t="s">
@@ -2274,9 +2270,7 @@
       <c r="M5" s="6">
         <v>4</v>
       </c>
-      <c r="N5" s="6">
-        <v>0</v>
-      </c>
+      <c r="N5" s="6"/>
     </row>
     <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6" s="7" t="s">
@@ -2318,9 +2312,7 @@
       <c r="M6" s="6">
         <v>5</v>
       </c>
-      <c r="N6" s="6">
-        <v>0</v>
-      </c>
+      <c r="N6" s="6"/>
     </row>
     <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7" s="7" t="s">
@@ -2362,9 +2354,7 @@
       <c r="M7" s="6">
         <v>6</v>
       </c>
-      <c r="N7" s="6">
-        <v>0</v>
-      </c>
+      <c r="N7" s="6"/>
     </row>
     <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
@@ -2406,9 +2396,7 @@
       <c r="M8" s="6">
         <v>7</v>
       </c>
-      <c r="N8" s="6">
-        <v>0</v>
-      </c>
+      <c r="N8" s="6"/>
     </row>
     <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
@@ -2450,9 +2438,7 @@
       <c r="M9" s="6">
         <v>8</v>
       </c>
-      <c r="N9" s="6">
-        <v>0</v>
-      </c>
+      <c r="N9" s="6"/>
     </row>
     <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10" s="7" t="s">
@@ -2494,9 +2480,7 @@
       <c r="M10" s="6">
         <v>9</v>
       </c>
-      <c r="N10" s="6">
-        <v>0</v>
-      </c>
+      <c r="N10" s="6"/>
     </row>
     <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11" s="7" t="s">
@@ -2538,9 +2522,7 @@
       <c r="M11" s="6">
         <v>0</v>
       </c>
-      <c r="N11" s="6">
-        <v>0</v>
-      </c>
+      <c r="N11" s="6"/>
     </row>
     <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12" s="7" t="s">
@@ -2582,9 +2564,7 @@
       <c r="M12" s="6">
         <v>1</v>
       </c>
-      <c r="N12" s="6">
-        <v>0</v>
-      </c>
+      <c r="N12" s="6"/>
     </row>
     <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13" s="7" t="s">
@@ -2626,9 +2606,7 @@
       <c r="M13" s="6">
         <v>2</v>
       </c>
-      <c r="N13" s="6">
-        <v>0</v>
-      </c>
+      <c r="N13" s="6"/>
     </row>
     <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14" s="7" t="s">
@@ -2670,9 +2648,7 @@
       <c r="M14" s="6">
         <v>3</v>
       </c>
-      <c r="N14" s="6">
-        <v>0</v>
-      </c>
+      <c r="N14" s="6"/>
     </row>
     <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15" s="7" t="s">
@@ -2714,9 +2690,7 @@
       <c r="M15" s="6">
         <v>4</v>
       </c>
-      <c r="N15" s="6">
-        <v>0</v>
-      </c>
+      <c r="N15" s="6"/>
     </row>
     <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16" s="7" t="s">
@@ -2758,9 +2732,7 @@
       <c r="M16" s="6">
         <v>5</v>
       </c>
-      <c r="N16" s="6">
-        <v>0</v>
-      </c>
+      <c r="N16" s="6"/>
     </row>
     <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17" s="7" t="s">
@@ -2802,9 +2774,7 @@
       <c r="M17" s="6">
         <v>6</v>
       </c>
-      <c r="N17" s="6">
-        <v>0</v>
-      </c>
+      <c r="N17" s="6"/>
     </row>
     <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18" s="7" t="s">
@@ -2846,9 +2816,7 @@
       <c r="M18" s="6">
         <v>7</v>
       </c>
-      <c r="N18" s="6">
-        <v>0</v>
-      </c>
+      <c r="N18" s="6"/>
     </row>
     <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19" s="7" t="s">
@@ -2890,9 +2858,7 @@
       <c r="M19" s="6">
         <v>8</v>
       </c>
-      <c r="N19" s="6">
-        <v>0</v>
-      </c>
+      <c r="N19" s="6"/>
     </row>
     <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20" s="7" t="s">
@@ -2934,9 +2900,7 @@
       <c r="M20" s="6">
         <v>9</v>
       </c>
-      <c r="N20" s="6">
-        <v>0</v>
-      </c>
+      <c r="N20" s="6"/>
     </row>
     <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21" s="7" t="s">
@@ -2978,9 +2942,7 @@
       <c r="M21" s="6">
         <v>1</v>
       </c>
-      <c r="N21" s="6">
-        <v>0</v>
-      </c>
+      <c r="N21" s="6"/>
     </row>
     <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22" s="7" t="s">
@@ -3022,9 +2984,7 @@
       <c r="M22" s="6">
         <v>2</v>
       </c>
-      <c r="N22" s="6">
-        <v>0</v>
-      </c>
+      <c r="N22" s="6"/>
     </row>
     <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23" s="7" t="s">
@@ -3066,9 +3026,7 @@
       <c r="M23" s="6">
         <v>3</v>
       </c>
-      <c r="N23" s="6">
-        <v>0</v>
-      </c>
+      <c r="N23" s="6"/>
     </row>
     <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24" s="7" t="s">
@@ -3110,9 +3068,7 @@
       <c r="M24" s="6">
         <v>4</v>
       </c>
-      <c r="N24" s="6">
-        <v>0</v>
-      </c>
+      <c r="N24" s="6"/>
     </row>
     <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25" s="7" t="s">
@@ -3154,9 +3110,7 @@
       <c r="M25" s="6">
         <v>0</v>
       </c>
-      <c r="N25" s="6">
-        <v>0</v>
-      </c>
+      <c r="N25" s="6"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26" s="7" t="s">
@@ -3198,9 +3152,7 @@
       <c r="M26" s="6">
         <v>5</v>
       </c>
-      <c r="N26" s="6">
-        <v>0</v>
-      </c>
+      <c r="N26" s="6"/>
     </row>
     <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27" s="7" t="s">
@@ -3240,9 +3192,7 @@
       <c r="M27" s="6">
         <v>6</v>
       </c>
-      <c r="N27" s="6">
-        <v>0</v>
-      </c>
+      <c r="N27" s="6"/>
     </row>
     <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28" s="7" t="s">
@@ -3284,9 +3234,7 @@
       <c r="M28" s="6">
         <v>7</v>
       </c>
-      <c r="N28" s="6">
-        <v>0</v>
-      </c>
+      <c r="N28" s="6"/>
     </row>
     <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29" s="7" t="s">
@@ -3328,9 +3276,7 @@
       <c r="M29" s="6">
         <v>8</v>
       </c>
-      <c r="N29" s="6">
-        <v>0</v>
-      </c>
+      <c r="N29" s="6"/>
     </row>
     <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30" s="7" t="s">
@@ -3372,9 +3318,7 @@
       <c r="M30" s="6">
         <v>9</v>
       </c>
-      <c r="N30" s="6">
-        <v>0</v>
-      </c>
+      <c r="N30" s="6"/>
     </row>
     <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31" s="7" t="s">
@@ -3416,9 +3360,7 @@
       <c r="M31" s="6">
         <v>0</v>
       </c>
-      <c r="N31" s="6">
-        <v>0</v>
-      </c>
+      <c r="N31" s="6"/>
     </row>
     <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32" s="7" t="s">
@@ -3460,9 +3402,7 @@
       <c r="M32" s="6">
         <v>1</v>
       </c>
-      <c r="N32" s="6">
-        <v>0</v>
-      </c>
+      <c r="N32" s="6"/>
     </row>
     <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33" s="7" t="s">
@@ -3504,9 +3444,7 @@
       <c r="M33" s="6">
         <v>2</v>
       </c>
-      <c r="N33" s="6">
-        <v>0</v>
-      </c>
+      <c r="N33" s="6"/>
     </row>
     <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34" s="7" t="s">
@@ -3548,9 +3486,7 @@
       <c r="M34" s="6">
         <v>3</v>
       </c>
-      <c r="N34" s="6">
-        <v>0</v>
-      </c>
+      <c r="N34" s="6"/>
     </row>
     <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35" s="7" t="s">
@@ -3592,9 +3528,7 @@
       <c r="M35" s="6">
         <v>4</v>
       </c>
-      <c r="N35" s="6">
-        <v>0</v>
-      </c>
+      <c r="N35" s="6"/>
     </row>
     <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36" s="7" t="s">
@@ -3636,9 +3570,7 @@
       <c r="M36" s="6">
         <v>5</v>
       </c>
-      <c r="N36" s="6">
-        <v>0</v>
-      </c>
+      <c r="N36" s="6"/>
     </row>
     <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37" s="7" t="s">
@@ -3680,9 +3612,7 @@
       <c r="M37" s="6">
         <v>6</v>
       </c>
-      <c r="N37" s="6">
-        <v>0</v>
-      </c>
+      <c r="N37" s="6"/>
     </row>
     <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38" s="7" t="s">
@@ -3724,9 +3654,7 @@
       <c r="M38" s="6">
         <v>7</v>
       </c>
-      <c r="N38" s="6">
-        <v>0</v>
-      </c>
+      <c r="N38" s="6"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39" s="7" t="s">
@@ -3768,9 +3696,7 @@
       <c r="M39" s="6">
         <v>8</v>
       </c>
-      <c r="N39" s="6">
-        <v>0</v>
-      </c>
+      <c r="N39" s="6"/>
     </row>
     <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40" s="7" t="s">
@@ -3812,9 +3738,7 @@
       <c r="M40" s="6">
         <v>9</v>
       </c>
-      <c r="N40" s="6">
-        <v>0</v>
-      </c>
+      <c r="N40" s="6"/>
     </row>
     <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41" s="7" t="s">
@@ -3856,9 +3780,7 @@
       <c r="M41" s="6">
         <v>0</v>
       </c>
-      <c r="N41" s="6">
-        <v>0</v>
-      </c>
+      <c r="N41" s="6"/>
     </row>
     <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42" s="7" t="s">
@@ -3900,9 +3822,7 @@
       <c r="M42" s="6">
         <v>1</v>
       </c>
-      <c r="N42" s="6">
-        <v>0</v>
-      </c>
+      <c r="N42" s="6"/>
     </row>
     <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43" s="7" t="s">
@@ -3944,9 +3864,7 @@
       <c r="M43" s="6">
         <v>2</v>
       </c>
-      <c r="N43" s="6">
-        <v>0</v>
-      </c>
+      <c r="N43" s="6"/>
     </row>
     <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44" s="7" t="s">
@@ -3988,9 +3906,7 @@
       <c r="M44" s="6">
         <v>3</v>
       </c>
-      <c r="N44" s="6">
-        <v>0</v>
-      </c>
+      <c r="N44" s="6"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45" s="7" t="s">
@@ -4032,9 +3948,7 @@
       <c r="M45" s="6">
         <v>4</v>
       </c>
-      <c r="N45" s="6">
-        <v>0</v>
-      </c>
+      <c r="N45" s="6"/>
     </row>
     <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46" s="7" t="s">
@@ -4076,9 +3990,7 @@
       <c r="M46" s="6">
         <v>5</v>
       </c>
-      <c r="N46" s="6">
-        <v>0</v>
-      </c>
+      <c r="N46" s="6"/>
     </row>
     <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47" s="7" t="s">
@@ -4120,9 +4032,7 @@
       <c r="M47" s="6">
         <v>6</v>
       </c>
-      <c r="N47" s="6">
-        <v>0</v>
-      </c>
+      <c r="N47" s="6"/>
     </row>
     <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48" s="7" t="s">
@@ -4164,9 +4074,7 @@
       <c r="M48" s="6">
         <v>7</v>
       </c>
-      <c r="N48" s="6">
-        <v>0</v>
-      </c>
+      <c r="N48" s="6"/>
     </row>
     <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49" s="7" t="s">
@@ -4208,9 +4116,7 @@
       <c r="M49" s="6">
         <v>8</v>
       </c>
-      <c r="N49" s="6">
-        <v>0</v>
-      </c>
+      <c r="N49" s="6"/>
     </row>
     <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50" s="7" t="s">
@@ -4252,9 +4158,7 @@
       <c r="M50" s="6">
         <v>9</v>
       </c>
-      <c r="N50" s="6">
-        <v>0</v>
-      </c>
+      <c r="N50" s="6"/>
     </row>
     <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51" s="7" t="s">
@@ -4296,9 +4200,7 @@
       <c r="M51" s="6">
         <v>0</v>
       </c>
-      <c r="N51" s="6">
-        <v>0</v>
-      </c>
+      <c r="N51" s="6"/>
     </row>
     <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52" s="7" t="s">
@@ -4340,9 +4242,7 @@
       <c r="M52" s="6">
         <v>1</v>
       </c>
-      <c r="N52" s="6">
-        <v>0</v>
-      </c>
+      <c r="N52" s="6"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53" s="7" t="s">
@@ -4384,9 +4284,7 @@
       <c r="M53" s="6">
         <v>2</v>
       </c>
-      <c r="N53" s="6">
-        <v>0</v>
-      </c>
+      <c r="N53" s="6"/>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54" s="7" t="s">
@@ -4428,9 +4326,7 @@
       <c r="M54" s="6">
         <v>3</v>
       </c>
-      <c r="N54" s="6">
-        <v>0</v>
-      </c>
+      <c r="N54" s="6"/>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55" s="7" t="s">
@@ -4472,9 +4368,7 @@
       <c r="M55" s="6">
         <v>4</v>
       </c>
-      <c r="N55" s="6">
-        <v>0</v>
-      </c>
+      <c r="N55" s="6"/>
     </row>
     <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56" s="7" t="s">
@@ -4516,9 +4410,7 @@
       <c r="M56" s="6">
         <v>5</v>
       </c>
-      <c r="N56" s="6">
-        <v>0</v>
-      </c>
+      <c r="N56" s="6"/>
     </row>
     <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57" s="7" t="s">
@@ -4560,9 +4452,7 @@
       <c r="M57" s="6">
         <v>6</v>
       </c>
-      <c r="N57" s="6">
-        <v>0</v>
-      </c>
+      <c r="N57" s="6"/>
     </row>
     <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58" s="7" t="s">
@@ -4604,9 +4494,7 @@
       <c r="M58" s="6">
         <v>7</v>
       </c>
-      <c r="N58" s="6">
-        <v>0</v>
-      </c>
+      <c r="N58" s="6"/>
     </row>
     <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59" s="7" t="s">
@@ -4648,9 +4536,7 @@
       <c r="M59" s="6">
         <v>8</v>
       </c>
-      <c r="N59" s="6">
-        <v>0</v>
-      </c>
+      <c r="N59" s="6"/>
     </row>
     <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60" s="7" t="s">
@@ -4692,9 +4578,7 @@
       <c r="M60" s="6">
         <v>9</v>
       </c>
-      <c r="N60" s="6">
-        <v>0</v>
-      </c>
+      <c r="N60" s="6"/>
     </row>
     <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61" s="7" t="s">
@@ -4736,9 +4620,7 @@
       <c r="M61" s="6">
         <v>0</v>
       </c>
-      <c r="N61" s="6">
-        <v>0</v>
-      </c>
+      <c r="N61" s="6"/>
     </row>
     <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62" s="7" t="s">
@@ -4780,9 +4662,7 @@
       <c r="M62" s="6">
         <v>1</v>
       </c>
-      <c r="N62" s="6">
-        <v>0</v>
-      </c>
+      <c r="N62" s="6"/>
     </row>
     <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63" s="7" t="s">
@@ -4824,9 +4704,7 @@
       <c r="M63" s="6">
         <v>2</v>
       </c>
-      <c r="N63" s="6">
-        <v>0</v>
-      </c>
+      <c r="N63" s="6"/>
     </row>
     <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64" s="7" t="s">
@@ -4868,9 +4746,7 @@
       <c r="M64" s="6">
         <v>3</v>
       </c>
-      <c r="N64" s="6">
-        <v>0</v>
-      </c>
+      <c r="N64" s="6"/>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65" s="7" t="s">
@@ -4912,9 +4788,7 @@
       <c r="M65" s="6">
         <v>4</v>
       </c>
-      <c r="N65" s="6">
-        <v>0</v>
-      </c>
+      <c r="N65" s="6"/>
     </row>
     <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66" s="7" t="s">
@@ -4956,9 +4830,7 @@
       <c r="M66" s="6">
         <v>5</v>
       </c>
-      <c r="N66" s="6">
-        <v>0</v>
-      </c>
+      <c r="N66" s="6"/>
     </row>
     <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67" s="7" t="s">
@@ -5000,9 +4872,7 @@
       <c r="M67" s="6">
         <v>6</v>
       </c>
-      <c r="N67" s="6">
-        <v>0</v>
-      </c>
+      <c r="N67" s="6"/>
     </row>
     <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68" s="7" t="s">
@@ -5044,9 +4914,7 @@
       <c r="M68" s="6">
         <v>7</v>
       </c>
-      <c r="N68" s="6">
-        <v>0</v>
-      </c>
+      <c r="N68" s="6"/>
     </row>
     <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69" s="7" t="s">
@@ -5088,9 +4956,7 @@
       <c r="M69" s="6">
         <v>8</v>
       </c>
-      <c r="N69" s="6">
-        <v>0</v>
-      </c>
+      <c r="N69" s="6"/>
     </row>
     <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70" s="7" t="s">
@@ -5132,9 +4998,7 @@
       <c r="M70" s="6">
         <v>9</v>
       </c>
-      <c r="N70" s="6">
-        <v>0</v>
-      </c>
+      <c r="N70" s="6"/>
     </row>
     <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71" s="7" t="s">
@@ -5176,9 +5040,7 @@
       <c r="M71" s="6">
         <v>0</v>
       </c>
-      <c r="N71" s="6">
-        <v>0</v>
-      </c>
+      <c r="N71" s="6"/>
     </row>
     <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72" s="7" t="s">
@@ -5220,9 +5082,7 @@
       <c r="M72" s="6">
         <v>1</v>
       </c>
-      <c r="N72" s="6">
-        <v>0</v>
-      </c>
+      <c r="N72" s="6"/>
     </row>
     <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73" s="7" t="s">
@@ -5264,9 +5124,7 @@
       <c r="M73" s="6">
         <v>2</v>
       </c>
-      <c r="N73" s="6">
-        <v>0</v>
-      </c>
+      <c r="N73" s="6"/>
     </row>
     <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74" s="7" t="s">
@@ -5308,9 +5166,7 @@
       <c r="M74" s="6">
         <v>3</v>
       </c>
-      <c r="N74" s="6">
-        <v>0</v>
-      </c>
+      <c r="N74" s="6"/>
     </row>
     <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75" s="7" t="s">
@@ -5352,9 +5208,7 @@
       <c r="M75" s="6">
         <v>4</v>
       </c>
-      <c r="N75" s="6">
-        <v>0</v>
-      </c>
+      <c r="N75" s="6"/>
     </row>
     <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76" s="7" t="s">
@@ -5396,9 +5250,7 @@
       <c r="M76" s="6">
         <v>5</v>
       </c>
-      <c r="N76" s="6">
-        <v>0</v>
-      </c>
+      <c r="N76" s="6"/>
     </row>
     <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77" s="7" t="s">
@@ -5440,9 +5292,7 @@
       <c r="M77" s="6">
         <v>6</v>
       </c>
-      <c r="N77" s="6">
-        <v>0</v>
-      </c>
+      <c r="N77" s="6"/>
     </row>
     <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78" s="7" t="s">
@@ -5484,9 +5334,7 @@
       <c r="M78" s="6">
         <v>7</v>
       </c>
-      <c r="N78" s="6">
-        <v>0</v>
-      </c>
+      <c r="N78" s="6"/>
     </row>
     <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79" s="7" t="s">
@@ -5528,9 +5376,7 @@
       <c r="M79" s="6">
         <v>8</v>
       </c>
-      <c r="N79" s="6">
-        <v>0</v>
-      </c>
+      <c r="N79" s="6"/>
     </row>
     <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80" s="7" t="s">
@@ -5572,9 +5418,7 @@
       <c r="M80" s="6">
         <v>9</v>
       </c>
-      <c r="N80" s="6">
-        <v>0</v>
-      </c>
+      <c r="N80" s="6"/>
     </row>
     <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81" s="7" t="s">
@@ -5616,9 +5460,7 @@
       <c r="M81" s="6">
         <v>0</v>
       </c>
-      <c r="N81" s="6">
-        <v>0</v>
-      </c>
+      <c r="N81" s="6"/>
     </row>
     <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82" s="7" t="s">
@@ -5660,9 +5502,7 @@
       <c r="M82" s="6">
         <v>1</v>
       </c>
-      <c r="N82" s="6">
-        <v>0</v>
-      </c>
+      <c r="N82" s="6"/>
     </row>
     <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83" s="7" t="s">
@@ -5704,9 +5544,7 @@
       <c r="M83" s="6">
         <v>2</v>
       </c>
-      <c r="N83" s="6">
-        <v>0</v>
-      </c>
+      <c r="N83" s="6"/>
     </row>
     <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84" s="7" t="s">
@@ -5748,9 +5586,7 @@
       <c r="M84" s="6">
         <v>4</v>
       </c>
-      <c r="N84" s="6">
-        <v>0</v>
-      </c>
+      <c r="N84" s="6"/>
     </row>
     <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85" s="7" t="s">
@@ -5792,9 +5628,7 @@
       <c r="M85" s="6">
         <v>5</v>
       </c>
-      <c r="N85" s="6">
-        <v>0</v>
-      </c>
+      <c r="N85" s="6"/>
     </row>
     <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86" s="7" t="s">
@@ -5836,9 +5670,7 @@
       <c r="M86" s="6">
         <v>6</v>
       </c>
-      <c r="N86" s="6">
-        <v>0</v>
-      </c>
+      <c r="N86" s="6"/>
     </row>
     <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87" s="7" t="s">
@@ -5880,9 +5712,7 @@
       <c r="M87" s="6">
         <v>7</v>
       </c>
-      <c r="N87" s="6">
-        <v>0</v>
-      </c>
+      <c r="N87" s="6"/>
     </row>
     <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88" s="7" t="s">
@@ -5924,9 +5754,7 @@
       <c r="M88" s="6">
         <v>8</v>
       </c>
-      <c r="N88" s="6">
-        <v>0</v>
-      </c>
+      <c r="N88" s="6"/>
     </row>
     <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89" s="7" t="s">
@@ -5968,9 +5796,7 @@
       <c r="M89" s="6">
         <v>9</v>
       </c>
-      <c r="N89" s="6">
-        <v>0</v>
-      </c>
+      <c r="N89" s="6"/>
     </row>
     <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90" s="7" t="s">
@@ -6012,9 +5838,7 @@
       <c r="M90" s="6">
         <v>0</v>
       </c>
-      <c r="N90" s="6">
-        <v>0</v>
-      </c>
+      <c r="N90" s="6"/>
     </row>
     <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91" s="7" t="s">
@@ -6056,9 +5880,7 @@
       <c r="M91" s="6">
         <v>1</v>
       </c>
-      <c r="N91" s="6">
-        <v>0</v>
-      </c>
+      <c r="N91" s="6"/>
     </row>
     <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92" s="7" t="s">
@@ -6100,9 +5922,7 @@
       <c r="M92" s="6">
         <v>2</v>
       </c>
-      <c r="N92" s="6">
-        <v>0</v>
-      </c>
+      <c r="N92" s="6"/>
     </row>
     <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93" s="7" t="s">
@@ -6144,9 +5964,7 @@
       <c r="M93" s="6">
         <v>3</v>
       </c>
-      <c r="N93" s="6">
-        <v>0</v>
-      </c>
+      <c r="N93" s="6"/>
     </row>
     <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94" s="7" t="s">
@@ -6188,9 +6006,7 @@
       <c r="M94" s="6">
         <v>4</v>
       </c>
-      <c r="N94" s="6">
-        <v>0</v>
-      </c>
+      <c r="N94" s="6"/>
     </row>
     <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95" s="7" t="s">
@@ -6232,9 +6048,7 @@
       <c r="M95" s="6">
         <v>4</v>
       </c>
-      <c r="N95" s="6">
-        <v>0</v>
-      </c>
+      <c r="N95" s="6"/>
     </row>
     <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96" s="7" t="s">
@@ -6276,9 +6090,7 @@
       <c r="M96" s="6">
         <v>5</v>
       </c>
-      <c r="N96" s="6">
-        <v>0</v>
-      </c>
+      <c r="N96" s="6"/>
     </row>
     <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97" s="7" t="s">
@@ -6320,9 +6132,7 @@
       <c r="M97" s="6">
         <v>6</v>
       </c>
-      <c r="N97" s="6">
-        <v>0</v>
-      </c>
+      <c r="N97" s="6"/>
     </row>
     <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98" s="7" t="s">
@@ -6364,9 +6174,7 @@
       <c r="M98" s="6">
         <v>7</v>
       </c>
-      <c r="N98" s="6">
-        <v>0</v>
-      </c>
+      <c r="N98" s="6"/>
     </row>
     <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99" s="7" t="s">
@@ -6408,9 +6216,7 @@
       <c r="M99" s="6">
         <v>8</v>
       </c>
-      <c r="N99" s="6">
-        <v>0</v>
-      </c>
+      <c r="N99" s="6"/>
     </row>
     <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100" s="7" t="s">
@@ -6452,9 +6258,7 @@
       <c r="M100" s="6">
         <v>9</v>
       </c>
-      <c r="N100" s="6">
-        <v>0</v>
-      </c>
+      <c r="N100" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>